<commit_message>
+ testing and OOAD labs
</commit_message>
<xml_diff>
--- a/Software implementation and testing/3/Чек-листы.xlsx
+++ b/Software implementation and testing/3/Чек-листы.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10390" yWindow="-120" windowWidth="12310" windowHeight="11390"/>
+    <workbookView xWindow="10400" yWindow="-120" windowWidth="12320" windowHeight="11390"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Тело сайта</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Проверить, что при нажатии на ссылку "Мои рассчёты" выплывает справа форма "Мои рассчёты"</t>
   </si>
   <si>
-    <t>Проверить, что при нажатии на жёлтую кнопку с иконкой звезды и надписью " В избранное" выплывает по середине предупреждение о необходимости регистрации</t>
-  </si>
-  <si>
     <t>Проверить наличие надписи "2015 – 2025 © calcus.ru. При использовании материалов сайта необходима ссылка на источник."</t>
   </si>
   <si>
@@ -119,50 +116,47 @@
     <t xml:space="preserve">Проверить, что при нажатии на иконку поиска появляется сверху форма "Поиск калькуляторов" </t>
   </si>
   <si>
-    <t>Проверить возможность ввода в поле ввода "Количество чисел" пробелов "  "</t>
-  </si>
-  <si>
-    <t>Проверить возможность ввода в поле ввода "Количество чисел" русских букв "абв"</t>
-  </si>
-  <si>
-    <t>Проверить возможность ввода в поле ввода "Количество чисел" букв латинского алфавита "abc"</t>
-  </si>
-  <si>
-    <t>Проверить возможность ввода в поля ввода диапазона спец символовов "*?-+"</t>
-  </si>
-  <si>
-    <t>Проверить возможность ввода в поле ввода "Количество чисел" спец символовов "*?-+"</t>
-  </si>
-  <si>
-    <t>Проверить возможность ввода в поля ввода диапазона букв латинского алфавита "abc"</t>
-  </si>
-  <si>
-    <t>Проверить возможность ввода в поля ввода "диапазона русских букв "абв"</t>
-  </si>
-  <si>
-    <t>Проверить возможность ввода в поля ввода диапазона пробелов "  "</t>
-  </si>
-  <si>
     <t>Проверить, что при нажатии кнопки "Генерировать", при незаполненных полях ввода "Количество чисел" и диапазона было предупреждение "Заполните это поле"</t>
   </si>
   <si>
     <t>Проверить, что при нажатии на кнопки увеличения и уменьшения количества чисел, расположенный справа от поля его ввода, количество либо увеличивается на 1, либо уменьшается соответственно</t>
   </si>
   <si>
-    <t>Проверить, что при нажатии на checkbox "Разрешить повторы", случайные числа могут повторяться</t>
-  </si>
-  <si>
-    <t>Проверить, что при нажатии на checkbox "Сортировать результат по порядку", случайные числа будут расположены от наименьшего к наибольшему</t>
-  </si>
-  <si>
     <t>сайт "https://calcus.ru/random-number"</t>
+  </si>
+  <si>
+    <t>Проверить невозможность ввода в поле ввода "Количество чисел" спец символовов "*?-+"</t>
+  </si>
+  <si>
+    <t>Проверить невозможность ввода в поле ввода "Количество чисел" пробелов "  "</t>
+  </si>
+  <si>
+    <t>Проверить невозможность ввода в поле ввода "Количество чисел" русских букв "абв"</t>
+  </si>
+  <si>
+    <t>Проверить невозможность ввода в поле ввода "Количество чисел" букв латинского алфавита "abc"</t>
+  </si>
+  <si>
+    <t>Проверить невозможность ввода в поля ввода диапазона спец символовов "*?-+"</t>
+  </si>
+  <si>
+    <t>Проверить невозможность ввода в поля ввода диапазона пробелов "  "</t>
+  </si>
+  <si>
+    <t>Проверить невозможность ввода в поля ввода диапазона букв латинского алфавита "abc"</t>
+  </si>
+  <si>
+    <t>Проверить невозможность ввода в поля ввода диапазона русских букв "абв"</t>
+  </si>
+  <si>
+    <t>Проверить, что при нажатии на жёлтую кнопку с иконкой звезды и надписью " В избранное" для неавторизованного пользователя выплывает по середине предупреждение о необходимости регистрации</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,13 +190,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -270,11 +290,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -290,9 +312,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -320,13 +339,21 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="3" builtinId="27"/>
+    <cellStyle name="Хороший" xfId="2" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -604,24 +631,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M74"/>
+  <dimension ref="A1:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="103.453125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.36328125" customWidth="1"/>
+    <col min="1" max="1" width="103.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.453125" customWidth="1"/>
     <col min="3" max="3" width="49.54296875" customWidth="1"/>
     <col min="4" max="4" width="48.453125" customWidth="1"/>
-    <col min="8" max="8" width="75.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="75.54296875" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -629,7 +656,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="13"/>
+      <c r="H1" s="12"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -645,7 +672,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I2" s="2"/>
@@ -655,7 +682,7 @@
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="2"/>
@@ -663,7 +690,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="11" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="2"/>
@@ -673,7 +700,7 @@
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="2"/>
@@ -681,7 +708,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="2"/>
@@ -691,15 +718,15 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
-        <v>30</v>
+      <c r="A5" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="B5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>17</v>
       </c>
       <c r="I5" s="2"/>
@@ -709,7 +736,7 @@
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="2"/>
@@ -717,7 +744,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="2"/>
@@ -736,7 +763,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="I7" s="2"/>
@@ -746,7 +773,7 @@
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2"/>
@@ -754,7 +781,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I8" s="2"/>
@@ -764,7 +791,7 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="2"/>
@@ -772,7 +799,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I9" s="2"/>
@@ -782,7 +809,7 @@
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="2"/>
@@ -790,7 +817,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I10" s="2"/>
@@ -800,15 +827,15 @@
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
-        <v>35</v>
+      <c r="A11" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="B11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I11" s="2"/>
@@ -818,15 +845,15 @@
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
-        <v>31</v>
+      <c r="A12" s="16" t="s">
+        <v>34</v>
       </c>
       <c r="B12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="12"/>
+      <c r="H12" s="11"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -834,15 +861,15 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
-        <v>32</v>
+      <c r="A13" s="16" t="s">
+        <v>35</v>
       </c>
       <c r="B13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="11" t="s">
         <v>12</v>
       </c>
       <c r="I13" s="2"/>
@@ -852,15 +879,15 @@
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
-        <v>33</v>
+      <c r="A14" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="B14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="15"/>
+      <c r="H14" s="14"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -868,15 +895,15 @@
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
-        <v>34</v>
+      <c r="A15" s="16" t="s">
+        <v>37</v>
       </c>
       <c r="B15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="15"/>
+      <c r="H15" s="14"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -884,15 +911,15 @@
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
-        <v>40</v>
+      <c r="A16" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="B16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="13"/>
+      <c r="H16" s="12"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -900,7 +927,7 @@
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="16" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="2"/>
@@ -908,7 +935,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="15"/>
+      <c r="H17" s="14"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -916,15 +943,15 @@
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
-        <v>37</v>
+      <c r="A18" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="B18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="15"/>
+      <c r="H18" s="14"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -932,15 +959,15 @@
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="7" t="s">
-        <v>36</v>
+      <c r="A19" s="16" t="s">
+        <v>39</v>
       </c>
       <c r="B19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="15"/>
+      <c r="H19" s="14"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -948,8 +975,8 @@
       <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="7" t="s">
-        <v>39</v>
+      <c r="A20" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="B20" s="2"/>
       <c r="D20" s="2"/>
@@ -963,7 +990,7 @@
       <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="2"/>
@@ -971,7 +998,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="13"/>
+      <c r="H21" s="12"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -979,7 +1006,7 @@
       <c r="M21" s="1"/>
     </row>
     <row r="22" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="2"/>
@@ -987,7 +1014,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="13"/>
+      <c r="H22" s="12"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -995,15 +1022,14 @@
       <c r="M22" s="1"/>
     </row>
     <row r="23" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="2"/>
+      <c r="A23" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="13"/>
+      <c r="H23" s="12"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -1011,19 +1037,29 @@
       <c r="M23" s="1"/>
     </row>
     <row r="24" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="A24" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="7" t="s">
-        <v>29</v>
+      <c r="A25" s="16" t="s">
+        <v>15</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="13"/>
+      <c r="H25" s="12"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -1031,14 +1067,14 @@
       <c r="M25" s="1"/>
     </row>
     <row r="26" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="7" t="s">
-        <v>26</v>
+      <c r="A26" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="13"/>
+      <c r="H26" s="12"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -1046,76 +1082,78 @@
       <c r="M26" s="1"/>
     </row>
     <row r="27" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="8" t="s">
-        <v>15</v>
-      </c>
+      <c r="A27" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="4"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="13"/>
+      <c r="H27" s="12"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="8" t="s">
-        <v>27</v>
+    <row r="28" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="16" t="s">
+        <v>11</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="13"/>
+      <c r="H28" s="12"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="4"/>
+    <row r="29" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="13"/>
+      <c r="H29" s="12"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="8" t="s">
-        <v>11</v>
-      </c>
+    <row r="30" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="13"/>
+      <c r="H30" s="12"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="6" t="s">
-        <v>18</v>
+    <row r="31" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="16" t="s">
+        <v>2</v>
       </c>
       <c r="B31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="13"/>
+      <c r="H31" s="12"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -1123,15 +1161,15 @@
       <c r="M31" s="1"/>
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="17" t="s">
-        <v>28</v>
+      <c r="A32" s="16" t="s">
+        <v>3</v>
       </c>
       <c r="B32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="13"/>
+      <c r="H32" s="12"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
@@ -1139,15 +1177,15 @@
       <c r="M32" s="1"/>
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="7" t="s">
-        <v>2</v>
+      <c r="A33" s="16" t="s">
+        <v>4</v>
       </c>
       <c r="B33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="13"/>
+      <c r="H33" s="12"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
@@ -1155,15 +1193,15 @@
       <c r="M33" s="1"/>
     </row>
     <row r="34" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="7" t="s">
-        <v>3</v>
+      <c r="A34" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="B34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="13"/>
+      <c r="H34" s="12"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
@@ -1171,15 +1209,13 @@
       <c r="M34" s="1"/>
     </row>
     <row r="35" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="7" t="s">
-        <v>4</v>
-      </c>
+      <c r="A35"/>
       <c r="B35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="13"/>
+      <c r="H35" s="12"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
@@ -1187,15 +1223,13 @@
       <c r="M35" s="1"/>
     </row>
     <row r="36" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="A36"/>
       <c r="B36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="13"/>
+      <c r="H36" s="12"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
@@ -1203,66 +1237,63 @@
       <c r="M36" s="1"/>
     </row>
     <row r="37" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37"/>
-      <c r="B37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
+      <c r="A37" s="8"/>
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38"/>
-      <c r="B38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
+      <c r="A38" s="8"/>
     </row>
     <row r="39" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="9"/>
+      <c r="A39" s="8"/>
     </row>
     <row r="40" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="9"/>
+      <c r="A40" s="8"/>
     </row>
     <row r="41" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="9"/>
+      <c r="A41" s="8"/>
     </row>
     <row r="42" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="9"/>
+      <c r="A42" s="8"/>
     </row>
     <row r="43" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="9"/>
+      <c r="A43" s="8"/>
     </row>
     <row r="44" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="9"/>
+      <c r="A44" s="8"/>
     </row>
     <row r="45" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="9"/>
+      <c r="A45" s="8"/>
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="9"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
     </row>
     <row r="47" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="9"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
     </row>
     <row r="48" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="3"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
-      <c r="H48" s="13"/>
+      <c r="H48" s="12"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
@@ -1270,11 +1301,12 @@
       <c r="M48" s="1"/>
     </row>
     <row r="49" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="3"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
-      <c r="H49" s="13"/>
+      <c r="H49" s="12"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
@@ -1287,7 +1319,7 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-      <c r="H50" s="13"/>
+      <c r="H50" s="12"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
@@ -1300,7 +1332,7 @@
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-      <c r="H51" s="13"/>
+      <c r="H51" s="12"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
@@ -1313,7 +1345,7 @@
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
-      <c r="H52" s="13"/>
+      <c r="H52" s="12"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
@@ -1326,7 +1358,7 @@
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
-      <c r="H53" s="13"/>
+      <c r="H53" s="12"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
@@ -1339,7 +1371,7 @@
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
-      <c r="H54" s="13"/>
+      <c r="H54" s="12"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
@@ -1352,7 +1384,7 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
-      <c r="H55" s="13"/>
+      <c r="H55" s="12"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -1360,12 +1392,12 @@
       <c r="M55" s="1"/>
     </row>
     <row r="56" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="3"/>
+      <c r="B56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
-      <c r="H56" s="13"/>
+      <c r="H56" s="12"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
@@ -1373,12 +1405,11 @@
       <c r="M56" s="1"/>
     </row>
     <row r="57" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="3"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
-      <c r="H57" s="13"/>
+      <c r="H57" s="12"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
@@ -1386,12 +1417,12 @@
       <c r="M57" s="1"/>
     </row>
     <row r="58" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="2"/>
+      <c r="B58" s="4"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
-      <c r="H58" s="13"/>
+      <c r="H58" s="12"/>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
@@ -1399,11 +1430,12 @@
       <c r="M58" s="1"/>
     </row>
     <row r="59" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
-      <c r="H59" s="13"/>
+      <c r="H59" s="12"/>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
@@ -1411,12 +1443,12 @@
       <c r="M59" s="1"/>
     </row>
     <row r="60" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="4"/>
+      <c r="B60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
-      <c r="H60" s="13"/>
+      <c r="H60" s="12"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
@@ -1429,7 +1461,7 @@
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
-      <c r="H61" s="13"/>
+      <c r="H61" s="12"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
@@ -1442,7 +1474,7 @@
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
-      <c r="H62" s="13"/>
+      <c r="H62" s="12"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
@@ -1455,7 +1487,7 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
-      <c r="H63" s="13"/>
+      <c r="H63" s="12"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
@@ -1468,7 +1500,7 @@
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-      <c r="H64" s="13"/>
+      <c r="H64" s="12"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
@@ -1481,7 +1513,7 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-      <c r="H65" s="13"/>
+      <c r="H65" s="12"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
@@ -1494,7 +1526,7 @@
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
-      <c r="H66" s="13"/>
+      <c r="H66" s="12"/>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
@@ -1507,7 +1539,7 @@
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
-      <c r="H67" s="13"/>
+      <c r="H67" s="12"/>
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
@@ -1520,7 +1552,7 @@
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
-      <c r="H68" s="13"/>
+      <c r="H68" s="12"/>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
@@ -1533,7 +1565,7 @@
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
-      <c r="H69" s="13"/>
+      <c r="H69" s="12"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
@@ -1546,7 +1578,7 @@
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
-      <c r="H70" s="13"/>
+      <c r="H70" s="12"/>
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
@@ -1559,7 +1591,7 @@
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
-      <c r="H71" s="13"/>
+      <c r="H71" s="12"/>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
@@ -1572,39 +1604,13 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
-      <c r="H72" s="13"/>
+      <c r="H72" s="12"/>
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
     </row>
-    <row r="73" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="13"/>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-      <c r="K73" s="2"/>
-      <c r="L73" s="1"/>
-      <c r="M73" s="1"/>
-    </row>
-    <row r="74" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-      <c r="G74" s="2"/>
-      <c r="H74" s="13"/>
-      <c r="I74" s="2"/>
-      <c r="J74" s="2"/>
-      <c r="K74" s="2"/>
-      <c r="L74" s="1"/>
-      <c r="M74" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
+7lab testing and some fixes
</commit_message>
<xml_diff>
--- a/Software implementation and testing/3/Чек-листы.xlsx
+++ b/Software implementation and testing/3/Чек-листы.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Seva\GitHub\TSU_TASKS\Software implementation and testing\3\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10400" yWindow="-120" windowWidth="12320" windowHeight="11390"/>
+    <workbookView xWindow="10395" yWindow="-120" windowWidth="12315" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -156,7 +151,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,39 +185,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -290,13 +259,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -312,6 +279,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -339,21 +309,13 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Плохой" xfId="3" builtinId="27"/>
-    <cellStyle name="Хороший" xfId="2" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -623,7 +585,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -631,22 +593,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M72"/>
+  <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="103.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.453125" customWidth="1"/>
-    <col min="3" max="3" width="49.54296875" customWidth="1"/>
-    <col min="4" max="4" width="48.453125" customWidth="1"/>
-    <col min="8" max="8" width="75.54296875" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="103.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" customWidth="1"/>
+    <col min="3" max="3" width="49.5703125" customWidth="1"/>
+    <col min="4" max="4" width="48.42578125" customWidth="1"/>
+    <col min="8" max="8" width="75.5703125" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>32</v>
       </c>
@@ -656,14 +618,14 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="12"/>
+      <c r="H1" s="13"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -672,7 +634,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="14" t="s">
         <v>16</v>
       </c>
       <c r="I2" s="2"/>
@@ -681,8 +643,8 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="2"/>
@@ -690,7 +652,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="12" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="2"/>
@@ -699,8 +661,8 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="2"/>
@@ -708,7 +670,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="2"/>
@@ -717,8 +679,8 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="2"/>
@@ -726,7 +688,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="14" t="s">
         <v>17</v>
       </c>
       <c r="I5" s="2"/>
@@ -735,8 +697,8 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="2"/>
@@ -744,7 +706,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="11" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="2"/>
@@ -753,7 +715,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>0</v>
       </c>
@@ -763,7 +725,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="8" t="s">
         <v>14</v>
       </c>
       <c r="I7" s="2"/>
@@ -772,8 +734,8 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
+    <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2"/>
@@ -781,7 +743,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I8" s="2"/>
@@ -790,8 +752,8 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="2"/>
@@ -799,7 +761,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I9" s="2"/>
@@ -808,8 +770,8 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
+    <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="2"/>
@@ -817,7 +779,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="8" t="s">
         <v>10</v>
       </c>
       <c r="I10" s="2"/>
@@ -826,8 +788,8 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="2"/>
@@ -835,7 +797,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="8" t="s">
         <v>11</v>
       </c>
       <c r="I11" s="2"/>
@@ -844,8 +806,8 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="16" t="s">
+    <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="2"/>
@@ -853,15 +815,15 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="11"/>
+      <c r="H12" s="12"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="2"/>
@@ -869,7 +831,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="I13" s="2"/>
@@ -878,8 +840,8 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="16" t="s">
+    <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="2"/>
@@ -887,15 +849,15 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="14"/>
+      <c r="H14" s="15"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="16" t="s">
+    <row r="15" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B15" s="2"/>
@@ -903,15 +865,15 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="14"/>
+      <c r="H15" s="15"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="16" t="s">
+    <row r="16" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="2"/>
@@ -919,15 +881,15 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="12"/>
+      <c r="H16" s="13"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="16" t="s">
+    <row r="17" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="2"/>
@@ -935,15 +897,15 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="14"/>
+      <c r="H17" s="15"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="16" t="s">
+    <row r="18" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B18" s="2"/>
@@ -951,15 +913,15 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="14"/>
+      <c r="H18" s="15"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="16" t="s">
+    <row r="19" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="2"/>
@@ -967,15 +929,15 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="14"/>
+      <c r="H19" s="15"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="16" t="s">
+    <row r="20" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="2"/>
@@ -989,8 +951,8 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="16" t="s">
+    <row r="21" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="2"/>
@@ -998,15 +960,15 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="12"/>
+      <c r="H21" s="13"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="16" t="s">
+    <row r="22" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="2"/>
@@ -1014,603 +976,620 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="12"/>
+      <c r="H22" s="13"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="16" t="s">
-        <v>28</v>
-      </c>
+    <row r="23" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="12"/>
+      <c r="H23" s="13"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="16" t="s">
-        <v>15</v>
+    <row r="24" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+    </row>
+    <row r="25" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="12"/>
+      <c r="H25" s="13"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="16" t="s">
-        <v>41</v>
+    <row r="26" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="12"/>
+      <c r="H26" s="13"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="4"/>
+    <row r="27" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="12"/>
+      <c r="H27" s="13"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="16" t="s">
-        <v>11</v>
+    <row r="28" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="12"/>
+      <c r="H28" s="13"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="2"/>
+    <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="4"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="12"/>
+      <c r="H29" s="13"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="2"/>
+    <row r="30" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="12"/>
+      <c r="H30" s="13"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="16" t="s">
-        <v>2</v>
+    <row r="31" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="B31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="12"/>
+      <c r="H31" s="13"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="16" t="s">
-        <v>3</v>
+    <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="B32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="12"/>
+      <c r="H32" s="13"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="16" t="s">
-        <v>4</v>
+    <row r="33" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="B33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="12"/>
+      <c r="H33" s="13"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="16" t="s">
-        <v>5</v>
+    <row r="34" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="B34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="12"/>
+      <c r="H34" s="13"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35"/>
+    <row r="35" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="B35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="12"/>
+      <c r="H35" s="13"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36"/>
+    <row r="36" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="B36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="12"/>
+      <c r="H36" s="13"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="8"/>
-    </row>
-    <row r="38" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="8"/>
-    </row>
-    <row r="39" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="8"/>
-    </row>
-    <row r="40" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="8"/>
-    </row>
-    <row r="41" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="8"/>
-    </row>
-    <row r="42" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="8"/>
-    </row>
-    <row r="43" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="8"/>
-    </row>
-    <row r="44" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="8"/>
-    </row>
-    <row r="45" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="8"/>
-    </row>
-    <row r="46" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-    </row>
-    <row r="47" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-    </row>
-    <row r="48" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="3"/>
+    <row r="37" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37"/>
+      <c r="B37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+    </row>
+    <row r="38" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38"/>
+      <c r="B38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+    </row>
+    <row r="39" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="9"/>
+    </row>
+    <row r="40" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="9"/>
+    </row>
+    <row r="41" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="9"/>
+    </row>
+    <row r="42" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="9"/>
+    </row>
+    <row r="43" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="9"/>
+    </row>
+    <row r="44" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="9"/>
+    </row>
+    <row r="45" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="9"/>
+    </row>
+    <row r="46" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="9"/>
+    </row>
+    <row r="47" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="9"/>
+    </row>
+    <row r="48" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
-      <c r="H48" s="12"/>
+      <c r="H48" s="13"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="3"/>
+    <row r="49" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
-      <c r="H49" s="12"/>
+      <c r="H49" s="13"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
     </row>
-    <row r="50" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="3"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-      <c r="H50" s="12"/>
+      <c r="H50" s="13"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
     </row>
-    <row r="51" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="3"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-      <c r="H51" s="12"/>
+      <c r="H51" s="13"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
     </row>
-    <row r="52" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="3"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
-      <c r="H52" s="12"/>
+      <c r="H52" s="13"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
     </row>
-    <row r="53" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="3"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
-      <c r="H53" s="12"/>
+      <c r="H53" s="13"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
     </row>
-    <row r="54" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="3"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
-      <c r="H54" s="12"/>
+      <c r="H54" s="13"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
     </row>
-    <row r="55" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="3"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
-      <c r="H55" s="12"/>
+      <c r="H55" s="13"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
     </row>
-    <row r="56" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="2"/>
+    <row r="56" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="3"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
-      <c r="H56" s="12"/>
+      <c r="H56" s="13"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
     </row>
-    <row r="57" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="3"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
-      <c r="H57" s="12"/>
+      <c r="H57" s="13"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
     </row>
-    <row r="58" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="4"/>
+    <row r="58" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
-      <c r="H58" s="12"/>
+      <c r="H58" s="13"/>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
     </row>
-    <row r="59" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="2"/>
+    <row r="59" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
-      <c r="H59" s="12"/>
+      <c r="H59" s="13"/>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
     </row>
-    <row r="60" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="2"/>
+    <row r="60" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="4"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
-      <c r="H60" s="12"/>
+      <c r="H60" s="13"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
     </row>
-    <row r="61" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
-      <c r="H61" s="12"/>
+      <c r="H61" s="13"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
     </row>
-    <row r="62" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
-      <c r="H62" s="12"/>
+      <c r="H62" s="13"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
     </row>
-    <row r="63" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
-      <c r="H63" s="12"/>
+      <c r="H63" s="13"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
     </row>
-    <row r="64" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-      <c r="H64" s="12"/>
+      <c r="H64" s="13"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
     </row>
-    <row r="65" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-      <c r="H65" s="12"/>
+      <c r="H65" s="13"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
     </row>
-    <row r="66" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
-      <c r="H66" s="12"/>
+      <c r="H66" s="13"/>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
     </row>
-    <row r="67" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
-      <c r="H67" s="12"/>
+      <c r="H67" s="13"/>
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
     </row>
-    <row r="68" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
-      <c r="H68" s="12"/>
+      <c r="H68" s="13"/>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
     </row>
-    <row r="69" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
-      <c r="H69" s="12"/>
+      <c r="H69" s="13"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
     </row>
-    <row r="70" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
-      <c r="H70" s="12"/>
+      <c r="H70" s="13"/>
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
     </row>
-    <row r="71" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
-      <c r="H71" s="12"/>
+      <c r="H71" s="13"/>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
     </row>
-    <row r="72" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
-      <c r="H72" s="12"/>
+      <c r="H72" s="13"/>
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
     </row>
+    <row r="73" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+    </row>
+    <row r="74" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>